<commit_message>
Finally it fetches the bu too
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drish\Python_Projects_And_Repos\Billscrape\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAD7A7-4377-40F7-BEA6-D55F56DF818B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -841,11 +847,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,7 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,32 +890,42 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf/>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
+      <numFmt numFmtId="6" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="6" formatCode="#,##0;[Red]\-#,##0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:D230" totalsRowShown="0">
-  <autoFilter ref="A1:D230"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:D230" totalsRowShown="0">
+  <autoFilter ref="A1:D230" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Provider" dataDxfId="0"/>
-    <tableColumn id="2" name="Mobile" dataDxfId="0"/>
-    <tableColumn id="3" name="₹ Amt." dataDxfId="1"/>
-    <tableColumn id="4" name="BU" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Provider"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mobile"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="₹ Amt." dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -950,7 +963,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -984,6 +997,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1018,9 +1032,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1193,14 +1208,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1224,9 +1247,9 @@
       <c r="C2" s="2">
         <v>99960</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1236,9 +1259,9 @@
       <c r="C3" s="2">
         <v>43330</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1248,9 +1271,9 @@
       <c r="C4" s="2">
         <v>12840</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1260,9 +1283,9 @@
       <c r="C5" s="2">
         <v>8080</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1272,9 +1295,9 @@
       <c r="C6" s="2">
         <v>48520</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1284,9 +1307,9 @@
       <c r="C7" s="2">
         <v>34390</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1296,9 +1319,9 @@
       <c r="C8" s="2">
         <v>9570</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1308,9 +1331,9 @@
       <c r="C9" s="2">
         <v>8170</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1320,9 +1343,9 @@
       <c r="C10" s="2">
         <v>379458</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1332,9 +1355,9 @@
       <c r="C11" s="2">
         <v>397122</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1344,9 +1367,9 @@
       <c r="C12" s="2">
         <v>317629</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1356,9 +1379,9 @@
       <c r="C13" s="2">
         <v>1263584</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1368,9 +1391,9 @@
       <c r="C14" s="2">
         <v>156417</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1380,9 +1403,9 @@
       <c r="C15" s="2">
         <v>117492</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1392,9 +1415,9 @@
       <c r="C16" s="2">
         <v>88390</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1404,9 +1427,9 @@
       <c r="C17" s="2">
         <v>62066</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1416,9 +1439,9 @@
       <c r="C18" s="2">
         <v>61732</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1428,9 +1451,9 @@
       <c r="C19" s="2">
         <v>225516</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,9 +1463,9 @@
       <c r="C20" s="2">
         <v>6306</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1452,9 +1475,9 @@
       <c r="C21" s="2">
         <v>518433</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1464,9 +1487,9 @@
       <c r="C22" s="2">
         <v>4517</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -1476,9 +1499,9 @@
       <c r="C23" s="2">
         <v>113893</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1488,9 +1511,9 @@
       <c r="C24" s="2">
         <v>2449</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1500,9 +1523,9 @@
       <c r="C25" s="2">
         <v>15870</v>
       </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1512,9 +1535,9 @@
       <c r="C26" s="2">
         <v>13576</v>
       </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1524,9 +1547,9 @@
       <c r="C27" s="2">
         <v>13569</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1536,9 +1559,9 @@
       <c r="C28" s="2">
         <v>8820</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -1548,9 +1571,9 @@
       <c r="C29" s="2">
         <v>4946</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1560,9 +1583,9 @@
       <c r="C30" s="2">
         <v>4887</v>
       </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1572,9 +1595,9 @@
       <c r="C31" s="2">
         <v>43288</v>
       </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -1584,9 +1607,9 @@
       <c r="C32" s="2">
         <v>162539</v>
       </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1596,9 +1619,9 @@
       <c r="C33" s="2">
         <v>97708</v>
       </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1608,9 +1631,9 @@
       <c r="C34" s="2">
         <v>133472</v>
       </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1620,9 +1643,9 @@
       <c r="C35" s="2">
         <v>14847</v>
       </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -1632,9 +1655,9 @@
       <c r="C36" s="2">
         <v>17820</v>
       </c>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1644,9 +1667,9 @@
       <c r="C37" s="2">
         <v>164140</v>
       </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
@@ -1656,9 +1679,9 @@
       <c r="C38" s="2">
         <v>153640</v>
       </c>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -1668,9 +1691,9 @@
       <c r="C39" s="2">
         <v>140150</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -1680,9 +1703,9 @@
       <c r="C40" s="2">
         <v>136060</v>
       </c>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1692,9 +1715,9 @@
       <c r="C41" s="2">
         <v>108380</v>
       </c>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -1704,9 +1727,9 @@
       <c r="C42" s="2">
         <v>106670</v>
       </c>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -1716,9 +1739,9 @@
       <c r="C43" s="2">
         <v>98580</v>
       </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -1728,9 +1751,9 @@
       <c r="C44" s="2">
         <v>97830</v>
       </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -1740,9 +1763,9 @@
       <c r="C45" s="2">
         <v>87410</v>
       </c>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
@@ -1752,9 +1775,9 @@
       <c r="C46" s="2">
         <v>136740</v>
       </c>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -1764,9 +1787,9 @@
       <c r="C47" s="2">
         <v>135760</v>
       </c>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -1776,9 +1799,9 @@
       <c r="C48" s="2">
         <v>73170</v>
       </c>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -1788,9 +1811,9 @@
       <c r="C49" s="2">
         <v>68240</v>
       </c>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,9 +1823,9 @@
       <c r="C50" s="2">
         <v>66570</v>
       </c>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -1812,9 +1835,9 @@
       <c r="C51" s="2">
         <v>47250</v>
       </c>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
@@ -1824,9 +1847,9 @@
       <c r="C52" s="2">
         <v>42300</v>
       </c>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -1836,9 +1859,9 @@
       <c r="C53" s="2">
         <v>2210</v>
       </c>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -1848,9 +1871,9 @@
       <c r="C54" s="2">
         <v>54530</v>
       </c>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -1860,9 +1883,9 @@
       <c r="C55" s="2">
         <v>49180</v>
       </c>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
@@ -1872,9 +1895,9 @@
       <c r="C56" s="2">
         <v>47880</v>
       </c>
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
@@ -1884,9 +1907,9 @@
       <c r="C57" s="2">
         <v>47510</v>
       </c>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>12</v>
       </c>
@@ -1896,9 +1919,9 @@
       <c r="C58" s="2">
         <v>43880</v>
       </c>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>12</v>
       </c>
@@ -1908,9 +1931,9 @@
       <c r="C59" s="2">
         <v>62740</v>
       </c>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
@@ -1920,9 +1943,9 @@
       <c r="C60" s="2">
         <v>130222</v>
       </c>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>13</v>
       </c>
@@ -1932,9 +1955,9 @@
       <c r="C61" s="2">
         <v>19820</v>
       </c>
-      <c r="D61" s="1"/>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
@@ -1944,9 +1967,9 @@
       <c r="C62" s="2">
         <v>18210</v>
       </c>
-      <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>13</v>
       </c>
@@ -1956,9 +1979,9 @@
       <c r="C63" s="2">
         <v>17089</v>
       </c>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>13</v>
       </c>
@@ -1968,9 +1991,9 @@
       <c r="C64" s="2">
         <v>13563</v>
       </c>
-      <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>13</v>
       </c>
@@ -1980,9 +2003,9 @@
       <c r="C65" s="2">
         <v>12886</v>
       </c>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>13</v>
       </c>
@@ -1992,9 +2015,9 @@
       <c r="C66" s="2">
         <v>4687</v>
       </c>
-      <c r="D66" s="1"/>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>13</v>
       </c>
@@ -2004,9 +2027,9 @@
       <c r="C67" s="2">
         <v>896</v>
       </c>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>13</v>
       </c>
@@ -2016,9 +2039,9 @@
       <c r="C68" s="2">
         <v>480</v>
       </c>
-      <c r="D68" s="1"/>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>14</v>
       </c>
@@ -2028,9 +2051,9 @@
       <c r="C69" s="2">
         <v>52814</v>
       </c>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -2040,9 +2063,9 @@
       <c r="C70" s="2">
         <v>31143</v>
       </c>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>14</v>
       </c>
@@ -2052,9 +2075,9 @@
       <c r="C71" s="2">
         <v>23487</v>
       </c>
-      <c r="D71" s="1"/>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>14</v>
       </c>
@@ -2064,9 +2087,9 @@
       <c r="C72" s="2">
         <v>11596</v>
       </c>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -2076,9 +2099,9 @@
       <c r="C73" s="2">
         <v>4119</v>
       </c>
-      <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
@@ -2088,9 +2111,9 @@
       <c r="C74" s="2">
         <v>395396</v>
       </c>
-      <c r="D74" s="1"/>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>14</v>
       </c>
@@ -2100,9 +2123,9 @@
       <c r="C75" s="2">
         <v>8485</v>
       </c>
-      <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>15</v>
       </c>
@@ -2112,9 +2135,9 @@
       <c r="C76" s="2">
         <v>68467</v>
       </c>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>15</v>
       </c>
@@ -2124,9 +2147,9 @@
       <c r="C77" s="2">
         <v>66801</v>
       </c>
-      <c r="D77" s="1"/>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>15</v>
       </c>
@@ -2136,9 +2159,9 @@
       <c r="C78" s="2">
         <v>29603</v>
       </c>
-      <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>15</v>
       </c>
@@ -2148,9 +2171,9 @@
       <c r="C79" s="2">
         <v>7494</v>
       </c>
-      <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>15</v>
       </c>
@@ -2160,9 +2183,9 @@
       <c r="C80" s="2">
         <v>1658</v>
       </c>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>15</v>
       </c>
@@ -2172,9 +2195,9 @@
       <c r="C81" s="2">
         <v>24</v>
       </c>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>15</v>
       </c>
@@ -2184,9 +2207,9 @@
       <c r="C82" s="2">
         <v>24</v>
       </c>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>15</v>
       </c>
@@ -2196,9 +2219,9 @@
       <c r="C83" s="2">
         <v>48075</v>
       </c>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>16</v>
       </c>
@@ -2208,9 +2231,9 @@
       <c r="C84" s="2">
         <v>316294</v>
       </c>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>16</v>
       </c>
@@ -2220,9 +2243,9 @@
       <c r="C85" s="2">
         <v>323932</v>
       </c>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>16</v>
       </c>
@@ -2232,9 +2255,9 @@
       <c r="C86" s="2">
         <v>133698</v>
       </c>
-      <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>16</v>
       </c>
@@ -2244,9 +2267,9 @@
       <c r="C87" s="2">
         <v>85457</v>
       </c>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>17</v>
       </c>
@@ -2256,9 +2279,9 @@
       <c r="C88" s="2">
         <v>68970</v>
       </c>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>17</v>
       </c>
@@ -2268,9 +2291,9 @@
       <c r="C89" s="2">
         <v>58611</v>
       </c>
-      <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>17</v>
       </c>
@@ -2280,9 +2303,9 @@
       <c r="C90" s="2">
         <v>55164</v>
       </c>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>17</v>
       </c>
@@ -2292,9 +2315,9 @@
       <c r="C91" s="2">
         <v>43759</v>
       </c>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>17</v>
       </c>
@@ -2304,9 +2327,9 @@
       <c r="C92" s="2">
         <v>43309</v>
       </c>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>17</v>
       </c>
@@ -2316,9 +2339,9 @@
       <c r="C93" s="2">
         <v>26980</v>
       </c>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>17</v>
       </c>
@@ -2328,9 +2351,9 @@
       <c r="C94" s="2">
         <v>26825</v>
       </c>
-      <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>17</v>
       </c>
@@ -2340,9 +2363,9 @@
       <c r="C95" s="2">
         <v>22274</v>
       </c>
-      <c r="D95" s="1"/>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>18</v>
       </c>
@@ -2352,9 +2375,9 @@
       <c r="C96" s="2">
         <v>4430</v>
       </c>
-      <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>19</v>
       </c>
@@ -2364,9 +2387,9 @@
       <c r="C97" s="2">
         <v>4073</v>
       </c>
-      <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>19</v>
       </c>
@@ -2376,9 +2399,9 @@
       <c r="C98" s="2">
         <v>1269</v>
       </c>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>20</v>
       </c>
@@ -2388,9 +2411,9 @@
       <c r="C99" s="2">
         <v>14041</v>
       </c>
-      <c r="D99" s="1"/>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>20</v>
       </c>
@@ -2400,9 +2423,9 @@
       <c r="C100" s="2">
         <v>180456</v>
       </c>
-      <c r="D100" s="1"/>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>20</v>
       </c>
@@ -2412,9 +2435,9 @@
       <c r="C101" s="2">
         <v>608366</v>
       </c>
-      <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>20</v>
       </c>
@@ -2424,9 +2447,9 @@
       <c r="C102" s="2">
         <v>3358</v>
       </c>
-      <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>20</v>
       </c>
@@ -2436,9 +2459,9 @@
       <c r="C103" s="2">
         <v>824652</v>
       </c>
-      <c r="D103" s="1"/>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>20</v>
       </c>
@@ -2448,9 +2471,9 @@
       <c r="C104" s="2">
         <v>668275</v>
       </c>
-      <c r="D104" s="1"/>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>20</v>
       </c>
@@ -2460,9 +2483,9 @@
       <c r="C105" s="2">
         <v>313454</v>
       </c>
-      <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>20</v>
       </c>
@@ -2472,9 +2495,9 @@
       <c r="C106" s="2">
         <v>248219</v>
       </c>
-      <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>20</v>
       </c>
@@ -2484,9 +2507,9 @@
       <c r="C107" s="2">
         <v>189164</v>
       </c>
-      <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>20</v>
       </c>
@@ -2496,9 +2519,9 @@
       <c r="C108" s="2">
         <v>171251</v>
       </c>
-      <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>21</v>
       </c>
@@ -2508,9 +2531,9 @@
       <c r="C109" s="2">
         <v>479976</v>
       </c>
-      <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>21</v>
       </c>
@@ -2520,9 +2543,9 @@
       <c r="C110" s="2">
         <v>577210</v>
       </c>
-      <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>21</v>
       </c>
@@ -2532,9 +2555,9 @@
       <c r="C111" s="2">
         <v>108050</v>
       </c>
-      <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>22</v>
       </c>
@@ -2544,9 +2567,9 @@
       <c r="C112" s="2">
         <v>2256695</v>
       </c>
-      <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>22</v>
       </c>
@@ -2556,9 +2579,9 @@
       <c r="C113" s="2">
         <v>1867855</v>
       </c>
-      <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>22</v>
       </c>
@@ -2568,9 +2591,9 @@
       <c r="C114" s="2">
         <v>1542632</v>
       </c>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>22</v>
       </c>
@@ -2580,9 +2603,9 @@
       <c r="C115" s="2">
         <v>978760</v>
       </c>
-      <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>22</v>
       </c>
@@ -2592,9 +2615,9 @@
       <c r="C116" s="2">
         <v>614602</v>
       </c>
-      <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>22</v>
       </c>
@@ -2604,9 +2627,9 @@
       <c r="C117" s="2">
         <v>583631</v>
       </c>
-      <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>22</v>
       </c>
@@ -2616,9 +2639,9 @@
       <c r="C118" s="2">
         <v>387790</v>
       </c>
-      <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>22</v>
       </c>
@@ -2628,9 +2651,9 @@
       <c r="C119" s="2">
         <v>359625</v>
       </c>
-      <c r="D119" s="1"/>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>22</v>
       </c>
@@ -2640,9 +2663,9 @@
       <c r="C120" s="2">
         <v>350336</v>
       </c>
-      <c r="D120" s="1"/>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>22</v>
       </c>
@@ -2652,9 +2675,9 @@
       <c r="C121" s="2">
         <v>233878</v>
       </c>
-      <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>23</v>
       </c>
@@ -2664,9 +2687,9 @@
       <c r="C122" s="2">
         <v>151849</v>
       </c>
-      <c r="D122" s="1"/>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>24</v>
       </c>
@@ -2676,9 +2699,9 @@
       <c r="C123" s="2">
         <v>131631</v>
       </c>
-      <c r="D123" s="1"/>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>24</v>
       </c>
@@ -2688,9 +2711,9 @@
       <c r="C124" s="2">
         <v>40142</v>
       </c>
-      <c r="D124" s="1"/>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>24</v>
       </c>
@@ -2700,9 +2723,9 @@
       <c r="C125" s="2">
         <v>30226</v>
       </c>
-      <c r="D125" s="1"/>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>24</v>
       </c>
@@ -2712,9 +2735,9 @@
       <c r="C126" s="2">
         <v>172672</v>
       </c>
-      <c r="D126" s="1"/>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>25</v>
       </c>
@@ -2724,9 +2747,9 @@
       <c r="C127" s="2">
         <v>85262</v>
       </c>
-      <c r="D127" s="1"/>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>25</v>
       </c>
@@ -2736,9 +2759,9 @@
       <c r="C128" s="2">
         <v>82152</v>
       </c>
-      <c r="D128" s="1"/>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>25</v>
       </c>
@@ -2748,9 +2771,9 @@
       <c r="C129" s="2">
         <v>81176</v>
       </c>
-      <c r="D129" s="1"/>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>25</v>
       </c>
@@ -2760,9 +2783,9 @@
       <c r="C130" s="2">
         <v>75844</v>
       </c>
-      <c r="D130" s="1"/>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>25</v>
       </c>
@@ -2772,9 +2795,9 @@
       <c r="C131" s="2">
         <v>62041</v>
       </c>
-      <c r="D131" s="1"/>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>25</v>
       </c>
@@ -2784,9 +2807,9 @@
       <c r="C132" s="2">
         <v>52838</v>
       </c>
-      <c r="D132" s="1"/>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>25</v>
       </c>
@@ -2796,9 +2819,9 @@
       <c r="C133" s="2">
         <v>47183</v>
       </c>
-      <c r="D133" s="1"/>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>25</v>
       </c>
@@ -2808,9 +2831,9 @@
       <c r="C134" s="2">
         <v>44385</v>
       </c>
-      <c r="D134" s="1"/>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>25</v>
       </c>
@@ -2820,9 +2843,9 @@
       <c r="C135" s="2">
         <v>39700</v>
       </c>
-      <c r="D135" s="1"/>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>25</v>
       </c>
@@ -2832,9 +2855,9 @@
       <c r="C136" s="2">
         <v>13336</v>
       </c>
-      <c r="D136" s="1"/>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>25</v>
       </c>
@@ -2844,9 +2867,9 @@
       <c r="C137" s="2">
         <v>36491</v>
       </c>
-      <c r="D137" s="1"/>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>25</v>
       </c>
@@ -2856,9 +2879,9 @@
       <c r="C138" s="2">
         <v>15076</v>
       </c>
-      <c r="D138" s="1"/>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>26</v>
       </c>
@@ -2868,9 +2891,11 @@
       <c r="C139" s="2">
         <v>283860</v>
       </c>
-      <c r="D139" s="1"/>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="D139" s="2">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>26</v>
       </c>
@@ -2880,9 +2905,11 @@
       <c r="C140" s="2">
         <v>125510</v>
       </c>
-      <c r="D140" s="1"/>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="D140" s="2">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>26</v>
       </c>
@@ -2892,9 +2919,11 @@
       <c r="C141" s="2">
         <v>118550</v>
       </c>
-      <c r="D141" s="1"/>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="D141" s="2">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>26</v>
       </c>
@@ -2904,9 +2933,11 @@
       <c r="C142" s="2">
         <v>116960</v>
       </c>
-      <c r="D142" s="1"/>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="D142" s="2">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>26</v>
       </c>
@@ -2916,9 +2947,11 @@
       <c r="C143" s="2">
         <v>36520</v>
       </c>
-      <c r="D143" s="1"/>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="D143" s="2">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>26</v>
       </c>
@@ -2928,9 +2961,11 @@
       <c r="C144" s="2">
         <v>14590</v>
       </c>
-      <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="D144" s="2">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>26</v>
       </c>
@@ -2940,9 +2975,11 @@
       <c r="C145" s="2">
         <v>2170</v>
       </c>
-      <c r="D145" s="1"/>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="D145" s="2">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>26</v>
       </c>
@@ -2952,9 +2989,11 @@
       <c r="C146" s="2">
         <v>209830</v>
       </c>
-      <c r="D146" s="1"/>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="D146" s="2">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>26</v>
       </c>
@@ -2964,9 +3003,11 @@
       <c r="C147" s="2">
         <v>102610</v>
       </c>
-      <c r="D147" s="1"/>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="D147" s="2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>26</v>
       </c>
@@ -2976,9 +3017,11 @@
       <c r="C148" s="2">
         <v>44440</v>
       </c>
-      <c r="D148" s="1"/>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="D148" s="2">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>26</v>
       </c>
@@ -2988,9 +3031,11 @@
       <c r="C149" s="2">
         <v>38440</v>
       </c>
-      <c r="D149" s="1"/>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="D149" s="2">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>27</v>
       </c>
@@ -3000,9 +3045,9 @@
       <c r="C150" s="2">
         <v>614980</v>
       </c>
-      <c r="D150" s="1"/>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>27</v>
       </c>
@@ -3012,9 +3057,9 @@
       <c r="C151" s="2">
         <v>402363</v>
       </c>
-      <c r="D151" s="1"/>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>27</v>
       </c>
@@ -3024,9 +3069,9 @@
       <c r="C152" s="2">
         <v>3403</v>
       </c>
-      <c r="D152" s="1"/>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>28</v>
       </c>
@@ -3036,9 +3081,9 @@
       <c r="C153" s="2">
         <v>357252</v>
       </c>
-      <c r="D153" s="1"/>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="D153" s="2"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>29</v>
       </c>
@@ -3048,9 +3093,9 @@
       <c r="C154" s="2">
         <v>72143</v>
       </c>
-      <c r="D154" s="1"/>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="D154" s="2"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>29</v>
       </c>
@@ -3060,9 +3105,9 @@
       <c r="C155" s="2">
         <v>57221</v>
       </c>
-      <c r="D155" s="1"/>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>29</v>
       </c>
@@ -3072,9 +3117,9 @@
       <c r="C156" s="2">
         <v>45963</v>
       </c>
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="D156" s="2"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>29</v>
       </c>
@@ -3084,9 +3129,9 @@
       <c r="C157" s="2">
         <v>162120</v>
       </c>
-      <c r="D157" s="1"/>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="D157" s="2"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>29</v>
       </c>
@@ -3096,9 +3141,9 @@
       <c r="C158" s="2">
         <v>47804</v>
       </c>
-      <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="D158" s="2"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>29</v>
       </c>
@@ -3108,9 +3153,9 @@
       <c r="C159" s="2">
         <v>11488</v>
       </c>
-      <c r="D159" s="1"/>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="D159" s="2"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>29</v>
       </c>
@@ -3120,9 +3165,9 @@
       <c r="C160" s="2">
         <v>33402</v>
       </c>
-      <c r="D160" s="1"/>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="D160" s="2"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>29</v>
       </c>
@@ -3132,9 +3177,9 @@
       <c r="C161" s="2">
         <v>71601</v>
       </c>
-      <c r="D161" s="1"/>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="D161" s="2"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>29</v>
       </c>
@@ -3144,9 +3189,9 @@
       <c r="C162" s="2">
         <v>44324</v>
       </c>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="D162" s="2"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>30</v>
       </c>
@@ -3156,9 +3201,9 @@
       <c r="C163" s="2">
         <v>397100</v>
       </c>
-      <c r="D163" s="1"/>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="D163" s="2"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>30</v>
       </c>
@@ -3168,9 +3213,9 @@
       <c r="C164" s="2">
         <v>269280</v>
       </c>
-      <c r="D164" s="1"/>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="D164" s="2"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>30</v>
       </c>
@@ -3180,9 +3225,9 @@
       <c r="C165" s="2">
         <v>517810</v>
       </c>
-      <c r="D165" s="1"/>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="D165" s="2"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>30</v>
       </c>
@@ -3192,9 +3237,9 @@
       <c r="C166" s="2">
         <v>15010</v>
       </c>
-      <c r="D166" s="1"/>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="D166" s="2"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>30</v>
       </c>
@@ -3204,9 +3249,9 @@
       <c r="C167" s="2">
         <v>8620</v>
       </c>
-      <c r="D167" s="1"/>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="D167" s="2"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>31</v>
       </c>
@@ -3216,9 +3261,9 @@
       <c r="C168" s="2">
         <v>56042</v>
       </c>
-      <c r="D168" s="1"/>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="D168" s="2"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>31</v>
       </c>
@@ -3228,9 +3273,9 @@
       <c r="C169" s="2">
         <v>42194</v>
       </c>
-      <c r="D169" s="1"/>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="D169" s="2"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>31</v>
       </c>
@@ -3240,9 +3285,9 @@
       <c r="C170" s="2">
         <v>23940</v>
       </c>
-      <c r="D170" s="1"/>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>32</v>
       </c>
@@ -3252,9 +3297,9 @@
       <c r="C171" s="2">
         <v>34666</v>
       </c>
-      <c r="D171" s="1"/>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="D171" s="2"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>32</v>
       </c>
@@ -3264,9 +3309,9 @@
       <c r="C172" s="2">
         <v>27974</v>
       </c>
-      <c r="D172" s="1"/>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>32</v>
       </c>
@@ -3276,9 +3321,9 @@
       <c r="C173" s="2">
         <v>27732</v>
       </c>
-      <c r="D173" s="1"/>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="D173" s="2"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>32</v>
       </c>
@@ -3288,9 +3333,9 @@
       <c r="C174" s="2">
         <v>26230</v>
       </c>
-      <c r="D174" s="1"/>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="D174" s="2"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>32</v>
       </c>
@@ -3300,9 +3345,9 @@
       <c r="C175" s="2">
         <v>29228</v>
       </c>
-      <c r="D175" s="1"/>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="D175" s="2"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>32</v>
       </c>
@@ -3312,9 +3357,9 @@
       <c r="C176" s="2">
         <v>33765</v>
       </c>
-      <c r="D176" s="1"/>
-    </row>
-    <row r="177" spans="1:4">
+      <c r="D176" s="2"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>33</v>
       </c>
@@ -3324,9 +3369,9 @@
       <c r="C177" s="2">
         <v>1869</v>
       </c>
-      <c r="D177" s="1"/>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="D177" s="2"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>34</v>
       </c>
@@ -3336,9 +3381,9 @@
       <c r="C178" s="2">
         <v>213801</v>
       </c>
-      <c r="D178" s="1"/>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>34</v>
       </c>
@@ -3348,9 +3393,9 @@
       <c r="C179" s="2">
         <v>445251</v>
       </c>
-      <c r="D179" s="1"/>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>34</v>
       </c>
@@ -3360,9 +3405,9 @@
       <c r="C180" s="2">
         <v>221224</v>
       </c>
-      <c r="D180" s="1"/>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>34</v>
       </c>
@@ -3372,9 +3417,9 @@
       <c r="C181" s="2">
         <v>199901</v>
       </c>
-      <c r="D181" s="1"/>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>34</v>
       </c>
@@ -3384,9 +3429,9 @@
       <c r="C182" s="2">
         <v>160571</v>
       </c>
-      <c r="D182" s="1"/>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>34</v>
       </c>
@@ -3396,9 +3441,9 @@
       <c r="C183" s="2">
         <v>151762</v>
       </c>
-      <c r="D183" s="1"/>
-    </row>
-    <row r="184" spans="1:4">
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>34</v>
       </c>
@@ -3408,9 +3453,9 @@
       <c r="C184" s="2">
         <v>126495</v>
       </c>
-      <c r="D184" s="1"/>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>34</v>
       </c>
@@ -3420,9 +3465,9 @@
       <c r="C185" s="2">
         <v>111923</v>
       </c>
-      <c r="D185" s="1"/>
-    </row>
-    <row r="186" spans="1:4">
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>34</v>
       </c>
@@ -3432,9 +3477,9 @@
       <c r="C186" s="2">
         <v>50530</v>
       </c>
-      <c r="D186" s="1"/>
-    </row>
-    <row r="187" spans="1:4">
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>34</v>
       </c>
@@ -3444,9 +3489,9 @@
       <c r="C187" s="2">
         <v>18278</v>
       </c>
-      <c r="D187" s="1"/>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>34</v>
       </c>
@@ -3456,9 +3501,9 @@
       <c r="C188" s="2">
         <v>90941</v>
       </c>
-      <c r="D188" s="1"/>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>35</v>
       </c>
@@ -3468,9 +3513,9 @@
       <c r="C189" s="2">
         <v>1251000</v>
       </c>
-      <c r="D189" s="1"/>
-    </row>
-    <row r="190" spans="1:4">
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>35</v>
       </c>
@@ -3480,9 +3525,9 @@
       <c r="C190" s="2">
         <v>76150</v>
       </c>
-      <c r="D190" s="1"/>
-    </row>
-    <row r="191" spans="1:4">
+      <c r="D190" s="2"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>35</v>
       </c>
@@ -3492,9 +3537,9 @@
       <c r="C191" s="2">
         <v>60840</v>
       </c>
-      <c r="D191" s="1"/>
-    </row>
-    <row r="192" spans="1:4">
+      <c r="D191" s="2"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>35</v>
       </c>
@@ -3504,9 +3549,9 @@
       <c r="C192" s="2">
         <v>56280</v>
       </c>
-      <c r="D192" s="1"/>
-    </row>
-    <row r="193" spans="1:4">
+      <c r="D192" s="2"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>35</v>
       </c>
@@ -3516,9 +3561,9 @@
       <c r="C193" s="2">
         <v>50290</v>
       </c>
-      <c r="D193" s="1"/>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>35</v>
       </c>
@@ -3528,9 +3573,9 @@
       <c r="C194" s="2">
         <v>68910</v>
       </c>
-      <c r="D194" s="1"/>
-    </row>
-    <row r="195" spans="1:4">
+      <c r="D194" s="2"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>35</v>
       </c>
@@ -3540,9 +3585,9 @@
       <c r="C195" s="2">
         <v>63600</v>
       </c>
-      <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="1:4">
+      <c r="D195" s="2"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>35</v>
       </c>
@@ -3552,9 +3597,9 @@
       <c r="C196" s="2">
         <v>52480</v>
       </c>
-      <c r="D196" s="1"/>
-    </row>
-    <row r="197" spans="1:4">
+      <c r="D196" s="2"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>35</v>
       </c>
@@ -3564,9 +3609,9 @@
       <c r="C197" s="2">
         <v>50270</v>
       </c>
-      <c r="D197" s="1"/>
-    </row>
-    <row r="198" spans="1:4">
+      <c r="D197" s="2"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>35</v>
       </c>
@@ -3576,9 +3621,9 @@
       <c r="C198" s="2">
         <v>45940</v>
       </c>
-      <c r="D198" s="1"/>
-    </row>
-    <row r="199" spans="1:4">
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>36</v>
       </c>
@@ -3588,9 +3633,9 @@
       <c r="C199" s="2">
         <v>7920</v>
       </c>
-      <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="1:4">
+      <c r="D199" s="2"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>36</v>
       </c>
@@ -3600,9 +3645,9 @@
       <c r="C200" s="2">
         <v>4300</v>
       </c>
-      <c r="D200" s="1"/>
-    </row>
-    <row r="201" spans="1:4">
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>36</v>
       </c>
@@ -3612,9 +3657,9 @@
       <c r="C201" s="2">
         <v>3390</v>
       </c>
-      <c r="D201" s="1"/>
-    </row>
-    <row r="202" spans="1:4">
+      <c r="D201" s="2"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>36</v>
       </c>
@@ -3624,9 +3669,9 @@
       <c r="C202" s="2">
         <v>1850</v>
       </c>
-      <c r="D202" s="1"/>
-    </row>
-    <row r="203" spans="1:4">
+      <c r="D202" s="2"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>36</v>
       </c>
@@ -3636,9 +3681,9 @@
       <c r="C203" s="2">
         <v>33480</v>
       </c>
-      <c r="D203" s="1"/>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="D203" s="2"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>37</v>
       </c>
@@ -3648,9 +3693,9 @@
       <c r="C204" s="2">
         <v>130585</v>
       </c>
-      <c r="D204" s="1"/>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>38</v>
       </c>
@@ -3660,9 +3705,9 @@
       <c r="C205" s="2">
         <v>1756</v>
       </c>
-      <c r="D205" s="1"/>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="D205" s="2"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>39</v>
       </c>
@@ -3672,9 +3717,9 @@
       <c r="C206" s="2">
         <v>105014</v>
       </c>
-      <c r="D206" s="1"/>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="D206" s="2"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>39</v>
       </c>
@@ -3684,9 +3729,9 @@
       <c r="C207" s="2">
         <v>97395</v>
       </c>
-      <c r="D207" s="1"/>
-    </row>
-    <row r="208" spans="1:4">
+      <c r="D207" s="2"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>39</v>
       </c>
@@ -3696,9 +3741,9 @@
       <c r="C208" s="2">
         <v>44217</v>
       </c>
-      <c r="D208" s="1"/>
-    </row>
-    <row r="209" spans="1:4">
+      <c r="D208" s="2"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>39</v>
       </c>
@@ -3708,9 +3753,9 @@
       <c r="C209" s="2">
         <v>4623</v>
       </c>
-      <c r="D209" s="1"/>
-    </row>
-    <row r="210" spans="1:4">
+      <c r="D209" s="2"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>40</v>
       </c>
@@ -3720,9 +3765,9 @@
       <c r="C210" s="2">
         <v>160144</v>
       </c>
-      <c r="D210" s="1"/>
-    </row>
-    <row r="211" spans="1:4">
+      <c r="D210" s="2"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>40</v>
       </c>
@@ -3732,9 +3777,9 @@
       <c r="C211" s="2">
         <v>104947</v>
       </c>
-      <c r="D211" s="1"/>
-    </row>
-    <row r="212" spans="1:4">
+      <c r="D211" s="2"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>41</v>
       </c>
@@ -3744,9 +3789,9 @@
       <c r="C212" s="2">
         <v>16001</v>
       </c>
-      <c r="D212" s="1"/>
-    </row>
-    <row r="213" spans="1:4">
+      <c r="D212" s="2"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>41</v>
       </c>
@@ -3756,9 +3801,9 @@
       <c r="C213" s="2">
         <v>14364</v>
       </c>
-      <c r="D213" s="1"/>
-    </row>
-    <row r="214" spans="1:4">
+      <c r="D213" s="2"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>41</v>
       </c>
@@ -3768,9 +3813,9 @@
       <c r="C214" s="2">
         <v>8508</v>
       </c>
-      <c r="D214" s="1"/>
-    </row>
-    <row r="215" spans="1:4">
+      <c r="D214" s="2"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>41</v>
       </c>
@@ -3780,9 +3825,9 @@
       <c r="C215" s="2">
         <v>6996</v>
       </c>
-      <c r="D215" s="1"/>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="D215" s="2"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>41</v>
       </c>
@@ -3792,9 +3837,9 @@
       <c r="C216" s="2">
         <v>6906</v>
       </c>
-      <c r="D216" s="1"/>
-    </row>
-    <row r="217" spans="1:4">
+      <c r="D216" s="2"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>41</v>
       </c>
@@ -3804,9 +3849,9 @@
       <c r="C217" s="2">
         <v>3022</v>
       </c>
-      <c r="D217" s="1"/>
-    </row>
-    <row r="218" spans="1:4">
+      <c r="D217" s="2"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>41</v>
       </c>
@@ -3816,9 +3861,9 @@
       <c r="C218" s="2">
         <v>3185</v>
       </c>
-      <c r="D218" s="1"/>
-    </row>
-    <row r="219" spans="1:4">
+      <c r="D218" s="2"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>42</v>
       </c>
@@ -3828,9 +3873,9 @@
       <c r="C219" s="2">
         <v>311627</v>
       </c>
-      <c r="D219" s="1"/>
-    </row>
-    <row r="220" spans="1:4">
+      <c r="D219" s="2"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>43</v>
       </c>
@@ -3840,9 +3885,9 @@
       <c r="C220" s="2">
         <v>124220</v>
       </c>
-      <c r="D220" s="1"/>
-    </row>
-    <row r="221" spans="1:4">
+      <c r="D220" s="2"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>43</v>
       </c>
@@ -3852,9 +3897,9 @@
       <c r="C221" s="2">
         <v>46850</v>
       </c>
-      <c r="D221" s="1"/>
-    </row>
-    <row r="222" spans="1:4">
+      <c r="D221" s="2"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>43</v>
       </c>
@@ -3864,9 +3909,9 @@
       <c r="C222" s="2">
         <v>29968</v>
       </c>
-      <c r="D222" s="1"/>
-    </row>
-    <row r="223" spans="1:4">
+      <c r="D222" s="2"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>43</v>
       </c>
@@ -3876,9 +3921,9 @@
       <c r="C223" s="2">
         <v>26764</v>
       </c>
-      <c r="D223" s="1"/>
-    </row>
-    <row r="224" spans="1:4">
+      <c r="D223" s="2"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>44</v>
       </c>
@@ -3888,9 +3933,9 @@
       <c r="C224" s="2">
         <v>141697</v>
       </c>
-      <c r="D224" s="1"/>
-    </row>
-    <row r="225" spans="1:4">
+      <c r="D224" s="2"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>44</v>
       </c>
@@ -3900,9 +3945,9 @@
       <c r="C225" s="2">
         <v>110073</v>
       </c>
-      <c r="D225" s="1"/>
-    </row>
-    <row r="226" spans="1:4">
+      <c r="D225" s="2"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>44</v>
       </c>
@@ -3912,9 +3957,9 @@
       <c r="C226" s="2">
         <v>101323</v>
       </c>
-      <c r="D226" s="1"/>
-    </row>
-    <row r="227" spans="1:4">
+      <c r="D226" s="2"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>44</v>
       </c>
@@ -3924,9 +3969,9 @@
       <c r="C227" s="2">
         <v>85192</v>
       </c>
-      <c r="D227" s="1"/>
-    </row>
-    <row r="228" spans="1:4">
+      <c r="D227" s="2"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>44</v>
       </c>
@@ -3936,9 +3981,9 @@
       <c r="C228" s="2">
         <v>66935</v>
       </c>
-      <c r="D228" s="1"/>
-    </row>
-    <row r="229" spans="1:4">
+      <c r="D228" s="2"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>44</v>
       </c>
@@ -3948,9 +3993,9 @@
       <c r="C229" s="2">
         <v>57705</v>
       </c>
-      <c r="D229" s="1"/>
-    </row>
-    <row r="230" spans="1:4">
+      <c r="D229" s="2"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>44</v>
       </c>
@@ -3960,7 +4005,7 @@
       <c r="C230" s="2">
         <v>57630</v>
       </c>
-      <c r="D230" s="1"/>
+      <c r="D230" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>